<commit_message>
ng: update site forms
</commit_message>
<xml_diff>
--- a/LF/TAS/Nigeria/2024/apr_2024/ng_lf_tas_202404_1_s_ben_oy.xlsx
+++ b/LF/TAS/Nigeria/2024/apr_2024/ng_lf_tas_202404_1_s_ben_oy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\LF\TAS\Nigeria\2024\apr_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B59F9900-7B8C-4667-8398-C036ADEA74FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2668DB1E-88C1-4B74-B09F-50318238E6EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3522" uniqueCount="532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3706" uniqueCount="532">
   <si>
     <t>type</t>
   </si>
@@ -1642,7 +1642,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="000"/>
+    <numFmt numFmtId="164" formatCode="000"/>
   </numFmts>
   <fonts count="10">
     <font>
@@ -1767,7 +1767,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1831,12 +1831,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2153,7 +2152,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D22" sqref="D22"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2556,9 +2555,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G710"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A231" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A254" sqref="A254:XFD259"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A665" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A526" sqref="A526:A710"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -10062,6 +10061,9 @@
       </c>
     </row>
     <row r="527" spans="1:6">
+      <c r="A527" t="s">
+        <v>89</v>
+      </c>
       <c r="B527" t="s">
         <v>214</v>
       </c>
@@ -10073,6 +10075,9 @@
       </c>
     </row>
     <row r="528" spans="1:6">
+      <c r="A528" t="s">
+        <v>89</v>
+      </c>
       <c r="B528" t="s">
         <v>70</v>
       </c>
@@ -10083,7 +10088,10 @@
         <v>217</v>
       </c>
     </row>
-    <row r="529" spans="2:6">
+    <row r="529" spans="1:6">
+      <c r="A529" t="s">
+        <v>89</v>
+      </c>
       <c r="B529" t="s">
         <v>77</v>
       </c>
@@ -10094,7 +10102,10 @@
         <v>218</v>
       </c>
     </row>
-    <row r="530" spans="2:6">
+    <row r="530" spans="1:6">
+      <c r="A530" t="s">
+        <v>89</v>
+      </c>
       <c r="B530">
         <v>113</v>
       </c>
@@ -10105,7 +10116,10 @@
         <v>220</v>
       </c>
     </row>
-    <row r="531" spans="2:6">
+    <row r="531" spans="1:6">
+      <c r="A531" t="s">
+        <v>89</v>
+      </c>
       <c r="B531" t="s">
         <v>221</v>
       </c>
@@ -10116,7 +10130,10 @@
         <v>222</v>
       </c>
     </row>
-    <row r="532" spans="2:6">
+    <row r="532" spans="1:6">
+      <c r="A532" t="s">
+        <v>89</v>
+      </c>
       <c r="B532" t="s">
         <v>82</v>
       </c>
@@ -10127,7 +10144,10 @@
         <v>224</v>
       </c>
     </row>
-    <row r="533" spans="2:6">
+    <row r="533" spans="1:6">
+      <c r="A533" t="s">
+        <v>89</v>
+      </c>
       <c r="B533" t="s">
         <v>84</v>
       </c>
@@ -10138,7 +10158,10 @@
         <v>226</v>
       </c>
     </row>
-    <row r="534" spans="2:6">
+    <row r="534" spans="1:6">
+      <c r="A534" t="s">
+        <v>89</v>
+      </c>
       <c r="B534" t="s">
         <v>71</v>
       </c>
@@ -10149,7 +10172,10 @@
         <v>228</v>
       </c>
     </row>
-    <row r="535" spans="2:6">
+    <row r="535" spans="1:6">
+      <c r="A535" t="s">
+        <v>89</v>
+      </c>
       <c r="B535" t="s">
         <v>144</v>
       </c>
@@ -10160,7 +10186,10 @@
         <v>230</v>
       </c>
     </row>
-    <row r="536" spans="2:6">
+    <row r="536" spans="1:6">
+      <c r="A536" t="s">
+        <v>89</v>
+      </c>
       <c r="B536" t="s">
         <v>200</v>
       </c>
@@ -10171,7 +10200,10 @@
         <v>232</v>
       </c>
     </row>
-    <row r="537" spans="2:6">
+    <row r="537" spans="1:6">
+      <c r="A537" t="s">
+        <v>89</v>
+      </c>
       <c r="B537" t="s">
         <v>165</v>
       </c>
@@ -10182,7 +10214,10 @@
         <v>529</v>
       </c>
     </row>
-    <row r="538" spans="2:6">
+    <row r="538" spans="1:6">
+      <c r="A538" t="s">
+        <v>89</v>
+      </c>
       <c r="B538">
         <v>108</v>
       </c>
@@ -10193,7 +10228,10 @@
         <v>235</v>
       </c>
     </row>
-    <row r="539" spans="2:6">
+    <row r="539" spans="1:6">
+      <c r="A539" t="s">
+        <v>89</v>
+      </c>
       <c r="B539">
         <v>126</v>
       </c>
@@ -10204,7 +10242,10 @@
         <v>237</v>
       </c>
     </row>
-    <row r="540" spans="2:6">
+    <row r="540" spans="1:6">
+      <c r="A540" t="s">
+        <v>89</v>
+      </c>
       <c r="B540">
         <v>144</v>
       </c>
@@ -10215,7 +10256,10 @@
         <v>238</v>
       </c>
     </row>
-    <row r="541" spans="2:6">
+    <row r="541" spans="1:6">
+      <c r="A541" t="s">
+        <v>89</v>
+      </c>
       <c r="B541">
         <v>161</v>
       </c>
@@ -10226,7 +10270,10 @@
         <v>240</v>
       </c>
     </row>
-    <row r="542" spans="2:6">
+    <row r="542" spans="1:6">
+      <c r="A542" t="s">
+        <v>89</v>
+      </c>
       <c r="B542">
         <v>179</v>
       </c>
@@ -10237,7 +10284,10 @@
         <v>242</v>
       </c>
     </row>
-    <row r="543" spans="2:6">
+    <row r="543" spans="1:6">
+      <c r="A543" t="s">
+        <v>89</v>
+      </c>
       <c r="B543">
         <v>197</v>
       </c>
@@ -10248,7 +10298,10 @@
         <v>244</v>
       </c>
     </row>
-    <row r="544" spans="2:6">
+    <row r="544" spans="1:6">
+      <c r="A544" t="s">
+        <v>89</v>
+      </c>
       <c r="B544">
         <v>215</v>
       </c>
@@ -10259,7 +10312,10 @@
         <v>246</v>
       </c>
     </row>
-    <row r="545" spans="2:6">
+    <row r="545" spans="1:6">
+      <c r="A545" t="s">
+        <v>89</v>
+      </c>
       <c r="B545">
         <v>233</v>
       </c>
@@ -10270,7 +10326,10 @@
         <v>248</v>
       </c>
     </row>
-    <row r="546" spans="2:6">
+    <row r="546" spans="1:6">
+      <c r="A546" t="s">
+        <v>89</v>
+      </c>
       <c r="B546">
         <v>251</v>
       </c>
@@ -10281,7 +10340,10 @@
         <v>250</v>
       </c>
     </row>
-    <row r="547" spans="2:6">
+    <row r="547" spans="1:6">
+      <c r="A547" t="s">
+        <v>89</v>
+      </c>
       <c r="B547">
         <v>268</v>
       </c>
@@ -10292,7 +10354,10 @@
         <v>462</v>
       </c>
     </row>
-    <row r="548" spans="2:6">
+    <row r="548" spans="1:6">
+      <c r="A548" t="s">
+        <v>89</v>
+      </c>
       <c r="B548">
         <v>286</v>
       </c>
@@ -10303,7 +10368,10 @@
         <v>463</v>
       </c>
     </row>
-    <row r="549" spans="2:6">
+    <row r="549" spans="1:6">
+      <c r="A549" t="s">
+        <v>89</v>
+      </c>
       <c r="B549">
         <v>304</v>
       </c>
@@ -10314,7 +10382,10 @@
         <v>464</v>
       </c>
     </row>
-    <row r="550" spans="2:6">
+    <row r="550" spans="1:6">
+      <c r="A550" t="s">
+        <v>89</v>
+      </c>
       <c r="B550">
         <v>322</v>
       </c>
@@ -10325,7 +10396,10 @@
         <v>465</v>
       </c>
     </row>
-    <row r="551" spans="2:6">
+    <row r="551" spans="1:6">
+      <c r="A551" t="s">
+        <v>89</v>
+      </c>
       <c r="B551">
         <v>340</v>
       </c>
@@ -10336,7 +10410,10 @@
         <v>255</v>
       </c>
     </row>
-    <row r="552" spans="2:6">
+    <row r="552" spans="1:6">
+      <c r="A552" t="s">
+        <v>89</v>
+      </c>
       <c r="B552">
         <v>358</v>
       </c>
@@ -10347,7 +10424,10 @@
         <v>466</v>
       </c>
     </row>
-    <row r="553" spans="2:6">
+    <row r="553" spans="1:6">
+      <c r="A553" t="s">
+        <v>89</v>
+      </c>
       <c r="B553">
         <v>375</v>
       </c>
@@ -10358,7 +10438,10 @@
         <v>467</v>
       </c>
     </row>
-    <row r="554" spans="2:6">
+    <row r="554" spans="1:6">
+      <c r="A554" t="s">
+        <v>89</v>
+      </c>
       <c r="B554">
         <v>393</v>
       </c>
@@ -10369,7 +10452,10 @@
         <v>468</v>
       </c>
     </row>
-    <row r="555" spans="2:6">
+    <row r="555" spans="1:6">
+      <c r="A555" t="s">
+        <v>89</v>
+      </c>
       <c r="B555">
         <v>411</v>
       </c>
@@ -10380,7 +10466,10 @@
         <v>469</v>
       </c>
     </row>
-    <row r="556" spans="2:6">
+    <row r="556" spans="1:6">
+      <c r="A556" t="s">
+        <v>89</v>
+      </c>
       <c r="B556">
         <v>429</v>
       </c>
@@ -10391,7 +10480,10 @@
         <v>470</v>
       </c>
     </row>
-    <row r="557" spans="2:6">
+    <row r="557" spans="1:6">
+      <c r="A557" t="s">
+        <v>89</v>
+      </c>
       <c r="B557">
         <v>447</v>
       </c>
@@ -10402,7 +10494,10 @@
         <v>471</v>
       </c>
     </row>
-    <row r="558" spans="2:6">
+    <row r="558" spans="1:6">
+      <c r="A558" t="s">
+        <v>89</v>
+      </c>
       <c r="B558">
         <v>465</v>
       </c>
@@ -10413,7 +10508,10 @@
         <v>472</v>
       </c>
     </row>
-    <row r="559" spans="2:6">
+    <row r="559" spans="1:6">
+      <c r="A559" t="s">
+        <v>89</v>
+      </c>
       <c r="B559">
         <v>482</v>
       </c>
@@ -10424,7 +10522,10 @@
         <v>473</v>
       </c>
     </row>
-    <row r="560" spans="2:6">
+    <row r="560" spans="1:6">
+      <c r="A560" t="s">
+        <v>89</v>
+      </c>
       <c r="B560">
         <v>500</v>
       </c>
@@ -10435,7 +10536,10 @@
         <v>474</v>
       </c>
     </row>
-    <row r="561" spans="2:6">
+    <row r="561" spans="1:6">
+      <c r="A561" t="s">
+        <v>89</v>
+      </c>
       <c r="B561">
         <v>518</v>
       </c>
@@ -10446,7 +10550,10 @@
         <v>265</v>
       </c>
     </row>
-    <row r="562" spans="2:6">
+    <row r="562" spans="1:6">
+      <c r="A562" t="s">
+        <v>89</v>
+      </c>
       <c r="B562">
         <v>132</v>
       </c>
@@ -10457,7 +10564,10 @@
         <v>267</v>
       </c>
     </row>
-    <row r="563" spans="2:6">
+    <row r="563" spans="1:6">
+      <c r="A563" t="s">
+        <v>89</v>
+      </c>
       <c r="B563">
         <v>417</v>
       </c>
@@ -10468,7 +10578,10 @@
         <v>475</v>
       </c>
     </row>
-    <row r="564" spans="2:6">
+    <row r="564" spans="1:6">
+      <c r="A564" t="s">
+        <v>89</v>
+      </c>
       <c r="B564">
         <v>167</v>
       </c>
@@ -10479,7 +10592,10 @@
         <v>270</v>
       </c>
     </row>
-    <row r="565" spans="2:6">
+    <row r="565" spans="1:6">
+      <c r="A565" t="s">
+        <v>89</v>
+      </c>
       <c r="B565">
         <v>488</v>
       </c>
@@ -10490,7 +10606,10 @@
         <v>476</v>
       </c>
     </row>
-    <row r="566" spans="2:6">
+    <row r="566" spans="1:6">
+      <c r="A566" t="s">
+        <v>89</v>
+      </c>
       <c r="B566">
         <v>274</v>
       </c>
@@ -10501,7 +10620,10 @@
         <v>477</v>
       </c>
     </row>
-    <row r="567" spans="2:6">
+    <row r="567" spans="1:6">
+      <c r="A567" t="s">
+        <v>89</v>
+      </c>
       <c r="B567">
         <v>310</v>
       </c>
@@ -10512,7 +10634,10 @@
         <v>478</v>
       </c>
     </row>
-    <row r="568" spans="2:6">
+    <row r="568" spans="1:6">
+      <c r="A568" t="s">
+        <v>89</v>
+      </c>
       <c r="B568">
         <v>239</v>
       </c>
@@ -10523,7 +10648,10 @@
         <v>275</v>
       </c>
     </row>
-    <row r="569" spans="2:6">
+    <row r="569" spans="1:6">
+      <c r="A569" t="s">
+        <v>89</v>
+      </c>
       <c r="B569" t="s">
         <v>277</v>
       </c>
@@ -10534,7 +10662,10 @@
         <v>278</v>
       </c>
     </row>
-    <row r="570" spans="2:6">
+    <row r="570" spans="1:6">
+      <c r="A570" t="s">
+        <v>89</v>
+      </c>
       <c r="B570" t="s">
         <v>78</v>
       </c>
@@ -10545,7 +10676,10 @@
         <v>280</v>
       </c>
     </row>
-    <row r="571" spans="2:6">
+    <row r="571" spans="1:6">
+      <c r="A571" t="s">
+        <v>89</v>
+      </c>
       <c r="B571" t="s">
         <v>168</v>
       </c>
@@ -10556,7 +10690,10 @@
         <v>281</v>
       </c>
     </row>
-    <row r="572" spans="2:6">
+    <row r="572" spans="1:6">
+      <c r="A572" t="s">
+        <v>89</v>
+      </c>
       <c r="B572">
         <v>203</v>
       </c>
@@ -10567,7 +10704,10 @@
         <v>282</v>
       </c>
     </row>
-    <row r="573" spans="2:6">
+    <row r="573" spans="1:6">
+      <c r="A573" t="s">
+        <v>89</v>
+      </c>
       <c r="B573">
         <v>524</v>
       </c>
@@ -10578,7 +10718,10 @@
         <v>479</v>
       </c>
     </row>
-    <row r="574" spans="2:6">
+    <row r="574" spans="1:6">
+      <c r="A574" t="s">
+        <v>89</v>
+      </c>
       <c r="B574">
         <v>453</v>
       </c>
@@ -10589,7 +10732,10 @@
         <v>480</v>
       </c>
     </row>
-    <row r="575" spans="2:6">
+    <row r="575" spans="1:6">
+      <c r="A575" t="s">
+        <v>89</v>
+      </c>
       <c r="B575">
         <v>346</v>
       </c>
@@ -10600,7 +10746,10 @@
         <v>481</v>
       </c>
     </row>
-    <row r="576" spans="2:6">
+    <row r="576" spans="1:6">
+      <c r="A576" t="s">
+        <v>89</v>
+      </c>
       <c r="B576">
         <v>381</v>
       </c>
@@ -10611,7 +10760,10 @@
         <v>482</v>
       </c>
     </row>
-    <row r="577" spans="2:6">
+    <row r="577" spans="1:6">
+      <c r="A577" t="s">
+        <v>89</v>
+      </c>
       <c r="B577">
         <v>2</v>
       </c>
@@ -10622,7 +10774,10 @@
         <v>483</v>
       </c>
     </row>
-    <row r="578" spans="2:6">
+    <row r="578" spans="1:6">
+      <c r="A578" t="s">
+        <v>89</v>
+      </c>
       <c r="B578">
         <v>5</v>
       </c>
@@ -10633,7 +10788,10 @@
         <v>484</v>
       </c>
     </row>
-    <row r="579" spans="2:6">
+    <row r="579" spans="1:6">
+      <c r="A579" t="s">
+        <v>89</v>
+      </c>
       <c r="B579">
         <v>9</v>
       </c>
@@ -10644,7 +10802,10 @@
         <v>288</v>
       </c>
     </row>
-    <row r="580" spans="2:6">
+    <row r="580" spans="1:6">
+      <c r="A580" t="s">
+        <v>89</v>
+      </c>
       <c r="B580">
         <v>12</v>
       </c>
@@ -10655,7 +10816,10 @@
         <v>485</v>
       </c>
     </row>
-    <row r="581" spans="2:6">
+    <row r="581" spans="1:6">
+      <c r="A581" t="s">
+        <v>89</v>
+      </c>
       <c r="B581">
         <v>15</v>
       </c>
@@ -10666,7 +10830,10 @@
         <v>486</v>
       </c>
     </row>
-    <row r="582" spans="2:6">
+    <row r="582" spans="1:6">
+      <c r="A582" t="s">
+        <v>89</v>
+      </c>
       <c r="B582">
         <v>18</v>
       </c>
@@ -10677,7 +10844,10 @@
         <v>487</v>
       </c>
     </row>
-    <row r="583" spans="2:6">
+    <row r="583" spans="1:6">
+      <c r="A583" t="s">
+        <v>89</v>
+      </c>
       <c r="B583">
         <v>21</v>
       </c>
@@ -10688,7 +10858,10 @@
         <v>488</v>
       </c>
     </row>
-    <row r="584" spans="2:6">
+    <row r="584" spans="1:6">
+      <c r="A584" t="s">
+        <v>89</v>
+      </c>
       <c r="B584">
         <v>24</v>
       </c>
@@ -10699,7 +10872,10 @@
         <v>489</v>
       </c>
     </row>
-    <row r="585" spans="2:6">
+    <row r="585" spans="1:6">
+      <c r="A585" t="s">
+        <v>89</v>
+      </c>
       <c r="B585">
         <v>28</v>
       </c>
@@ -10710,7 +10886,10 @@
         <v>490</v>
       </c>
     </row>
-    <row r="586" spans="2:6">
+    <row r="586" spans="1:6">
+      <c r="A586" t="s">
+        <v>89</v>
+      </c>
       <c r="B586">
         <v>31</v>
       </c>
@@ -10721,7 +10900,10 @@
         <v>491</v>
       </c>
     </row>
-    <row r="587" spans="2:6">
+    <row r="587" spans="1:6">
+      <c r="A587" t="s">
+        <v>89</v>
+      </c>
       <c r="B587">
         <v>34</v>
       </c>
@@ -10732,7 +10914,10 @@
         <v>297</v>
       </c>
     </row>
-    <row r="588" spans="2:6">
+    <row r="588" spans="1:6">
+      <c r="A588" t="s">
+        <v>89</v>
+      </c>
       <c r="B588">
         <v>37</v>
       </c>
@@ -10743,7 +10928,10 @@
         <v>492</v>
       </c>
     </row>
-    <row r="589" spans="2:6">
+    <row r="589" spans="1:6">
+      <c r="A589" t="s">
+        <v>89</v>
+      </c>
       <c r="B589">
         <v>40</v>
       </c>
@@ -10754,7 +10942,10 @@
         <v>298</v>
       </c>
     </row>
-    <row r="590" spans="2:6">
+    <row r="590" spans="1:6">
+      <c r="A590" t="s">
+        <v>89</v>
+      </c>
       <c r="B590">
         <v>43</v>
       </c>
@@ -10765,7 +10956,10 @@
         <v>300</v>
       </c>
     </row>
-    <row r="591" spans="2:6">
+    <row r="591" spans="1:6">
+      <c r="A591" t="s">
+        <v>89</v>
+      </c>
       <c r="B591">
         <v>47</v>
       </c>
@@ -10776,7 +10970,10 @@
         <v>493</v>
       </c>
     </row>
-    <row r="592" spans="2:6">
+    <row r="592" spans="1:6">
+      <c r="A592" t="s">
+        <v>89</v>
+      </c>
       <c r="B592">
         <v>50</v>
       </c>
@@ -10787,7 +10984,10 @@
         <v>494</v>
       </c>
     </row>
-    <row r="593" spans="2:6">
+    <row r="593" spans="1:6">
+      <c r="A593" t="s">
+        <v>89</v>
+      </c>
       <c r="B593">
         <v>53</v>
       </c>
@@ -10798,7 +10998,10 @@
         <v>304</v>
       </c>
     </row>
-    <row r="594" spans="2:6">
+    <row r="594" spans="1:6">
+      <c r="A594" t="s">
+        <v>89</v>
+      </c>
       <c r="B594">
         <v>56</v>
       </c>
@@ -10809,7 +11012,10 @@
         <v>306</v>
       </c>
     </row>
-    <row r="595" spans="2:6">
+    <row r="595" spans="1:6">
+      <c r="A595" t="s">
+        <v>89</v>
+      </c>
       <c r="B595">
         <v>59</v>
       </c>
@@ -10820,7 +11026,10 @@
         <v>308</v>
       </c>
     </row>
-    <row r="596" spans="2:6">
+    <row r="596" spans="1:6">
+      <c r="A596" t="s">
+        <v>89</v>
+      </c>
       <c r="B596">
         <v>62</v>
       </c>
@@ -10831,7 +11040,10 @@
         <v>310</v>
       </c>
     </row>
-    <row r="597" spans="2:6">
+    <row r="597" spans="1:6">
+      <c r="A597" t="s">
+        <v>89</v>
+      </c>
       <c r="B597">
         <v>66</v>
       </c>
@@ -10842,7 +11054,10 @@
         <v>311</v>
       </c>
     </row>
-    <row r="598" spans="2:6">
+    <row r="598" spans="1:6">
+      <c r="A598" t="s">
+        <v>89</v>
+      </c>
       <c r="B598">
         <v>69</v>
       </c>
@@ -10853,7 +11068,10 @@
         <v>312</v>
       </c>
     </row>
-    <row r="599" spans="2:6">
+    <row r="599" spans="1:6">
+      <c r="A599" t="s">
+        <v>89</v>
+      </c>
       <c r="B599">
         <v>72</v>
       </c>
@@ -10864,7 +11082,10 @@
         <v>313</v>
       </c>
     </row>
-    <row r="600" spans="2:6">
+    <row r="600" spans="1:6">
+      <c r="A600" t="s">
+        <v>89</v>
+      </c>
       <c r="B600">
         <v>75</v>
       </c>
@@ -10875,7 +11096,10 @@
         <v>314</v>
       </c>
     </row>
-    <row r="601" spans="2:6">
+    <row r="601" spans="1:6">
+      <c r="A601" t="s">
+        <v>89</v>
+      </c>
       <c r="B601">
         <v>78</v>
       </c>
@@ -10886,7 +11110,10 @@
         <v>495</v>
       </c>
     </row>
-    <row r="602" spans="2:6">
+    <row r="602" spans="1:6">
+      <c r="A602" t="s">
+        <v>89</v>
+      </c>
       <c r="B602">
         <v>81</v>
       </c>
@@ -10897,7 +11124,10 @@
         <v>315</v>
       </c>
     </row>
-    <row r="603" spans="2:6">
+    <row r="603" spans="1:6">
+      <c r="A603" t="s">
+        <v>89</v>
+      </c>
       <c r="B603">
         <v>85</v>
       </c>
@@ -10908,7 +11138,10 @@
         <v>316</v>
       </c>
     </row>
-    <row r="604" spans="2:6">
+    <row r="604" spans="1:6">
+      <c r="A604" t="s">
+        <v>89</v>
+      </c>
       <c r="B604">
         <v>88</v>
       </c>
@@ -10919,7 +11152,10 @@
         <v>317</v>
       </c>
     </row>
-    <row r="605" spans="2:6">
+    <row r="605" spans="1:6">
+      <c r="A605" t="s">
+        <v>89</v>
+      </c>
       <c r="B605">
         <v>91</v>
       </c>
@@ -10930,7 +11166,10 @@
         <v>318</v>
       </c>
     </row>
-    <row r="606" spans="2:6">
+    <row r="606" spans="1:6">
+      <c r="A606" t="s">
+        <v>89</v>
+      </c>
       <c r="B606">
         <v>94</v>
       </c>
@@ -10941,7 +11180,10 @@
         <v>319</v>
       </c>
     </row>
-    <row r="607" spans="2:6">
+    <row r="607" spans="1:6">
+      <c r="A607" t="s">
+        <v>89</v>
+      </c>
       <c r="B607">
         <v>61</v>
       </c>
@@ -10952,7 +11194,10 @@
         <v>320</v>
       </c>
     </row>
-    <row r="608" spans="2:6">
+    <row r="608" spans="1:6">
+      <c r="A608" t="s">
+        <v>89</v>
+      </c>
       <c r="B608">
         <v>80</v>
       </c>
@@ -10963,7 +11208,10 @@
         <v>321</v>
       </c>
     </row>
-    <row r="609" spans="2:6">
+    <row r="609" spans="1:6">
+      <c r="A609" t="s">
+        <v>89</v>
+      </c>
       <c r="B609">
         <v>4</v>
       </c>
@@ -10974,7 +11222,10 @@
         <v>322</v>
       </c>
     </row>
-    <row r="610" spans="2:6">
+    <row r="610" spans="1:6">
+      <c r="A610" t="s">
+        <v>89</v>
+      </c>
       <c r="B610">
         <v>17</v>
       </c>
@@ -10985,7 +11236,10 @@
         <v>324</v>
       </c>
     </row>
-    <row r="611" spans="2:6">
+    <row r="611" spans="1:6">
+      <c r="A611" t="s">
+        <v>89</v>
+      </c>
       <c r="B611">
         <v>36</v>
       </c>
@@ -10996,7 +11250,10 @@
         <v>326</v>
       </c>
     </row>
-    <row r="612" spans="2:6">
+    <row r="612" spans="1:6">
+      <c r="A612" t="s">
+        <v>89</v>
+      </c>
       <c r="B612">
         <v>74</v>
       </c>
@@ -11007,7 +11264,10 @@
         <v>327</v>
       </c>
     </row>
-    <row r="613" spans="2:6">
+    <row r="613" spans="1:6">
+      <c r="A613" t="s">
+        <v>89</v>
+      </c>
       <c r="B613">
         <v>10</v>
       </c>
@@ -11018,7 +11278,10 @@
         <v>496</v>
       </c>
     </row>
-    <row r="614" spans="2:6">
+    <row r="614" spans="1:6">
+      <c r="A614" t="s">
+        <v>89</v>
+      </c>
       <c r="B614">
         <v>29</v>
       </c>
@@ -11029,7 +11292,10 @@
         <v>497</v>
       </c>
     </row>
-    <row r="615" spans="2:6">
+    <row r="615" spans="1:6">
+      <c r="A615" t="s">
+        <v>89</v>
+      </c>
       <c r="B615">
         <v>93</v>
       </c>
@@ -11040,7 +11306,10 @@
         <v>330</v>
       </c>
     </row>
-    <row r="616" spans="2:6">
+    <row r="616" spans="1:6">
+      <c r="A616" t="s">
+        <v>89</v>
+      </c>
       <c r="B616">
         <v>23</v>
       </c>
@@ -11051,7 +11320,10 @@
         <v>331</v>
       </c>
     </row>
-    <row r="617" spans="2:6">
+    <row r="617" spans="1:6">
+      <c r="A617" t="s">
+        <v>89</v>
+      </c>
       <c r="B617">
         <v>55</v>
       </c>
@@ -11062,7 +11334,10 @@
         <v>498</v>
       </c>
     </row>
-    <row r="618" spans="2:6">
+    <row r="618" spans="1:6">
+      <c r="A618" t="s">
+        <v>89</v>
+      </c>
       <c r="B618">
         <v>42</v>
       </c>
@@ -11073,7 +11348,10 @@
         <v>334</v>
       </c>
     </row>
-    <row r="619" spans="2:6">
+    <row r="619" spans="1:6">
+      <c r="A619" t="s">
+        <v>89</v>
+      </c>
       <c r="B619">
         <v>48</v>
       </c>
@@ -11084,7 +11362,10 @@
         <v>499</v>
       </c>
     </row>
-    <row r="620" spans="2:6">
+    <row r="620" spans="1:6">
+      <c r="A620" t="s">
+        <v>89</v>
+      </c>
       <c r="B620">
         <v>67</v>
       </c>
@@ -11095,7 +11376,10 @@
         <v>337</v>
       </c>
     </row>
-    <row r="621" spans="2:6">
+    <row r="621" spans="1:6">
+      <c r="A621" t="s">
+        <v>89</v>
+      </c>
       <c r="B621">
         <v>86</v>
       </c>
@@ -11106,7 +11390,10 @@
         <v>338</v>
       </c>
     </row>
-    <row r="622" spans="2:6">
+    <row r="622" spans="1:6">
+      <c r="A622" t="s">
+        <v>89</v>
+      </c>
       <c r="B622">
         <v>1</v>
       </c>
@@ -11117,7 +11404,10 @@
         <v>339</v>
       </c>
     </row>
-    <row r="623" spans="2:6">
+    <row r="623" spans="1:6">
+      <c r="A623" t="s">
+        <v>89</v>
+      </c>
       <c r="B623">
         <v>3</v>
       </c>
@@ -11128,7 +11418,10 @@
         <v>341</v>
       </c>
     </row>
-    <row r="624" spans="2:6">
+    <row r="624" spans="1:6">
+      <c r="A624" t="s">
+        <v>89</v>
+      </c>
       <c r="B624">
         <v>5</v>
       </c>
@@ -11139,7 +11432,10 @@
         <v>343</v>
       </c>
     </row>
-    <row r="625" spans="2:6">
+    <row r="625" spans="1:6">
+      <c r="A625" t="s">
+        <v>89</v>
+      </c>
       <c r="B625">
         <v>7</v>
       </c>
@@ -11150,7 +11446,10 @@
         <v>344</v>
       </c>
     </row>
-    <row r="626" spans="2:6">
+    <row r="626" spans="1:6">
+      <c r="A626" t="s">
+        <v>89</v>
+      </c>
       <c r="B626">
         <v>10</v>
       </c>
@@ -11161,7 +11460,10 @@
         <v>346</v>
       </c>
     </row>
-    <row r="627" spans="2:6">
+    <row r="627" spans="1:6">
+      <c r="A627" t="s">
+        <v>89</v>
+      </c>
       <c r="B627">
         <v>12</v>
       </c>
@@ -11172,7 +11474,10 @@
         <v>348</v>
       </c>
     </row>
-    <row r="628" spans="2:6">
+    <row r="628" spans="1:6">
+      <c r="A628" t="s">
+        <v>89</v>
+      </c>
       <c r="B628">
         <v>14</v>
       </c>
@@ -11183,7 +11488,10 @@
         <v>525</v>
       </c>
     </row>
-    <row r="629" spans="2:6">
+    <row r="629" spans="1:6">
+      <c r="A629" t="s">
+        <v>89</v>
+      </c>
       <c r="B629">
         <v>16</v>
       </c>
@@ -11194,7 +11502,10 @@
         <v>351</v>
       </c>
     </row>
-    <row r="630" spans="2:6">
+    <row r="630" spans="1:6">
+      <c r="A630" t="s">
+        <v>89</v>
+      </c>
       <c r="B630">
         <v>19</v>
       </c>
@@ -11205,7 +11516,10 @@
         <v>353</v>
       </c>
     </row>
-    <row r="631" spans="2:6">
+    <row r="631" spans="1:6">
+      <c r="A631" t="s">
+        <v>89</v>
+      </c>
       <c r="B631">
         <v>21</v>
       </c>
@@ -11216,7 +11530,10 @@
         <v>355</v>
       </c>
     </row>
-    <row r="632" spans="2:6">
+    <row r="632" spans="1:6">
+      <c r="A632" t="s">
+        <v>89</v>
+      </c>
       <c r="B632">
         <v>23</v>
       </c>
@@ -11227,7 +11544,10 @@
         <v>357</v>
       </c>
     </row>
-    <row r="633" spans="2:6">
+    <row r="633" spans="1:6">
+      <c r="A633" t="s">
+        <v>89</v>
+      </c>
       <c r="B633">
         <v>25</v>
       </c>
@@ -11238,7 +11558,10 @@
         <v>359</v>
       </c>
     </row>
-    <row r="634" spans="2:6">
+    <row r="634" spans="1:6">
+      <c r="A634" t="s">
+        <v>89</v>
+      </c>
       <c r="B634">
         <v>28</v>
       </c>
@@ -11249,7 +11572,10 @@
         <v>361</v>
       </c>
     </row>
-    <row r="635" spans="2:6">
+    <row r="635" spans="1:6">
+      <c r="A635" t="s">
+        <v>89</v>
+      </c>
       <c r="B635">
         <v>30</v>
       </c>
@@ -11260,7 +11586,10 @@
         <v>362</v>
       </c>
     </row>
-    <row r="636" spans="2:6">
+    <row r="636" spans="1:6">
+      <c r="A636" t="s">
+        <v>89</v>
+      </c>
       <c r="B636">
         <v>32</v>
       </c>
@@ -11271,7 +11600,10 @@
         <v>364</v>
       </c>
     </row>
-    <row r="637" spans="2:6">
+    <row r="637" spans="1:6">
+      <c r="A637" t="s">
+        <v>89</v>
+      </c>
       <c r="B637">
         <v>34</v>
       </c>
@@ -11282,7 +11614,10 @@
         <v>500</v>
       </c>
     </row>
-    <row r="638" spans="2:6">
+    <row r="638" spans="1:6">
+      <c r="A638" t="s">
+        <v>89</v>
+      </c>
       <c r="B638">
         <v>36</v>
       </c>
@@ -11293,7 +11628,10 @@
         <v>367</v>
       </c>
     </row>
-    <row r="639" spans="2:6">
+    <row r="639" spans="1:6">
+      <c r="A639" t="s">
+        <v>89</v>
+      </c>
       <c r="B639">
         <v>39</v>
       </c>
@@ -11304,7 +11642,10 @@
         <v>369</v>
       </c>
     </row>
-    <row r="640" spans="2:6">
+    <row r="640" spans="1:6">
+      <c r="A640" t="s">
+        <v>89</v>
+      </c>
       <c r="B640">
         <v>41</v>
       </c>
@@ -11315,7 +11656,10 @@
         <v>527</v>
       </c>
     </row>
-    <row r="641" spans="2:6">
+    <row r="641" spans="1:6">
+      <c r="A641" t="s">
+        <v>89</v>
+      </c>
       <c r="B641">
         <v>43</v>
       </c>
@@ -11326,7 +11670,10 @@
         <v>371</v>
       </c>
     </row>
-    <row r="642" spans="2:6">
+    <row r="642" spans="1:6">
+      <c r="A642" t="s">
+        <v>89</v>
+      </c>
       <c r="B642">
         <v>45</v>
       </c>
@@ -11337,7 +11684,10 @@
         <v>373</v>
       </c>
     </row>
-    <row r="643" spans="2:6">
+    <row r="643" spans="1:6">
+      <c r="A643" t="s">
+        <v>89</v>
+      </c>
       <c r="B643">
         <v>48</v>
       </c>
@@ -11348,7 +11698,10 @@
         <v>374</v>
       </c>
     </row>
-    <row r="644" spans="2:6">
+    <row r="644" spans="1:6">
+      <c r="A644" t="s">
+        <v>89</v>
+      </c>
       <c r="B644">
         <v>50</v>
       </c>
@@ -11359,7 +11712,10 @@
         <v>376</v>
       </c>
     </row>
-    <row r="645" spans="2:6">
+    <row r="645" spans="1:6">
+      <c r="A645" t="s">
+        <v>89</v>
+      </c>
       <c r="B645">
         <v>52</v>
       </c>
@@ -11370,7 +11726,10 @@
         <v>378</v>
       </c>
     </row>
-    <row r="646" spans="2:6">
+    <row r="646" spans="1:6">
+      <c r="A646" t="s">
+        <v>89</v>
+      </c>
       <c r="B646">
         <v>54</v>
       </c>
@@ -11381,7 +11740,10 @@
         <v>380</v>
       </c>
     </row>
-    <row r="647" spans="2:6">
+    <row r="647" spans="1:6">
+      <c r="A647" t="s">
+        <v>89</v>
+      </c>
       <c r="B647">
         <v>57</v>
       </c>
@@ -11392,7 +11754,10 @@
         <v>382</v>
       </c>
     </row>
-    <row r="648" spans="2:6">
+    <row r="648" spans="1:6">
+      <c r="A648" t="s">
+        <v>89</v>
+      </c>
       <c r="B648">
         <v>59</v>
       </c>
@@ -11403,7 +11768,10 @@
         <v>384</v>
       </c>
     </row>
-    <row r="649" spans="2:6">
+    <row r="649" spans="1:6">
+      <c r="A649" t="s">
+        <v>89</v>
+      </c>
       <c r="B649">
         <v>61</v>
       </c>
@@ -11414,7 +11782,10 @@
         <v>385</v>
       </c>
     </row>
-    <row r="650" spans="2:6">
+    <row r="650" spans="1:6">
+      <c r="A650" t="s">
+        <v>89</v>
+      </c>
       <c r="B650">
         <v>63</v>
       </c>
@@ -11425,7 +11796,10 @@
         <v>386</v>
       </c>
     </row>
-    <row r="651" spans="2:6">
+    <row r="651" spans="1:6">
+      <c r="A651" t="s">
+        <v>89</v>
+      </c>
       <c r="B651">
         <v>66</v>
       </c>
@@ -11436,7 +11810,10 @@
         <v>501</v>
       </c>
     </row>
-    <row r="652" spans="2:6">
+    <row r="652" spans="1:6">
+      <c r="A652" t="s">
+        <v>89</v>
+      </c>
       <c r="B652">
         <v>8</v>
       </c>
@@ -11447,7 +11824,10 @@
         <v>389</v>
       </c>
     </row>
-    <row r="653" spans="2:6">
+    <row r="653" spans="1:6">
+      <c r="A653" t="s">
+        <v>89</v>
+      </c>
       <c r="B653">
         <v>38</v>
       </c>
@@ -11458,7 +11838,10 @@
         <v>391</v>
       </c>
     </row>
-    <row r="654" spans="2:6">
+    <row r="654" spans="1:6">
+      <c r="A654" t="s">
+        <v>89</v>
+      </c>
       <c r="B654">
         <v>17</v>
       </c>
@@ -11469,7 +11852,10 @@
         <v>392</v>
       </c>
     </row>
-    <row r="655" spans="2:6">
+    <row r="655" spans="1:6">
+      <c r="A655" t="s">
+        <v>89</v>
+      </c>
       <c r="B655">
         <v>60</v>
       </c>
@@ -11480,7 +11866,10 @@
         <v>393</v>
       </c>
     </row>
-    <row r="656" spans="2:6">
+    <row r="656" spans="1:6">
+      <c r="A656" t="s">
+        <v>89</v>
+      </c>
       <c r="B656">
         <v>29</v>
       </c>
@@ -11491,7 +11880,10 @@
         <v>395</v>
       </c>
     </row>
-    <row r="657" spans="2:6">
+    <row r="657" spans="1:6">
+      <c r="A657" t="s">
+        <v>89</v>
+      </c>
       <c r="B657">
         <v>11</v>
       </c>
@@ -11502,7 +11894,10 @@
         <v>397</v>
       </c>
     </row>
-    <row r="658" spans="2:6">
+    <row r="658" spans="1:6">
+      <c r="A658" t="s">
+        <v>89</v>
+      </c>
       <c r="B658">
         <v>51</v>
       </c>
@@ -11513,7 +11908,10 @@
         <v>399</v>
       </c>
     </row>
-    <row r="659" spans="2:6">
+    <row r="659" spans="1:6">
+      <c r="A659" t="s">
+        <v>89</v>
+      </c>
       <c r="B659">
         <v>56</v>
       </c>
@@ -11524,7 +11922,10 @@
         <v>400</v>
       </c>
     </row>
-    <row r="660" spans="2:6">
+    <row r="660" spans="1:6">
+      <c r="A660" t="s">
+        <v>89</v>
+      </c>
       <c r="B660">
         <v>42</v>
       </c>
@@ -11535,7 +11936,10 @@
         <v>402</v>
       </c>
     </row>
-    <row r="661" spans="2:6">
+    <row r="661" spans="1:6">
+      <c r="A661" t="s">
+        <v>89</v>
+      </c>
       <c r="B661">
         <v>20</v>
       </c>
@@ -11546,7 +11950,10 @@
         <v>404</v>
       </c>
     </row>
-    <row r="662" spans="2:6">
+    <row r="662" spans="1:6">
+      <c r="A662" t="s">
+        <v>89</v>
+      </c>
       <c r="B662">
         <v>35</v>
       </c>
@@ -11557,7 +11964,10 @@
         <v>526</v>
       </c>
     </row>
-    <row r="663" spans="2:6">
+    <row r="663" spans="1:6">
+      <c r="A663" t="s">
+        <v>89</v>
+      </c>
       <c r="B663">
         <v>65</v>
       </c>
@@ -11568,7 +11978,10 @@
         <v>502</v>
       </c>
     </row>
-    <row r="664" spans="2:6">
+    <row r="664" spans="1:6">
+      <c r="A664" t="s">
+        <v>89</v>
+      </c>
       <c r="B664">
         <v>26</v>
       </c>
@@ -11579,7 +11992,10 @@
         <v>406</v>
       </c>
     </row>
-    <row r="665" spans="2:6">
+    <row r="665" spans="1:6">
+      <c r="A665" t="s">
+        <v>89</v>
+      </c>
       <c r="B665">
         <v>2</v>
       </c>
@@ -11590,7 +12006,10 @@
         <v>528</v>
       </c>
     </row>
-    <row r="666" spans="2:6">
+    <row r="666" spans="1:6">
+      <c r="A666" t="s">
+        <v>89</v>
+      </c>
       <c r="B666">
         <v>47</v>
       </c>
@@ -11601,7 +12020,10 @@
         <v>408</v>
       </c>
     </row>
-    <row r="667" spans="2:6">
+    <row r="667" spans="1:6">
+      <c r="A667" t="s">
+        <v>89</v>
+      </c>
       <c r="B667">
         <v>1</v>
       </c>
@@ -11612,7 +12034,10 @@
         <v>410</v>
       </c>
     </row>
-    <row r="668" spans="2:6">
+    <row r="668" spans="1:6">
+      <c r="A668" t="s">
+        <v>89</v>
+      </c>
       <c r="B668">
         <v>4</v>
       </c>
@@ -11623,7 +12048,10 @@
         <v>412</v>
       </c>
     </row>
-    <row r="669" spans="2:6">
+    <row r="669" spans="1:6">
+      <c r="A669" t="s">
+        <v>89</v>
+      </c>
       <c r="B669">
         <v>8</v>
       </c>
@@ -11634,7 +12062,10 @@
         <v>413</v>
       </c>
     </row>
-    <row r="670" spans="2:6">
+    <row r="670" spans="1:6">
+      <c r="A670" t="s">
+        <v>89</v>
+      </c>
       <c r="B670">
         <v>11</v>
       </c>
@@ -11645,7 +12076,10 @@
         <v>414</v>
       </c>
     </row>
-    <row r="671" spans="2:6">
+    <row r="671" spans="1:6">
+      <c r="A671" t="s">
+        <v>89</v>
+      </c>
       <c r="B671">
         <v>14</v>
       </c>
@@ -11656,7 +12090,10 @@
         <v>415</v>
       </c>
     </row>
-    <row r="672" spans="2:6">
+    <row r="672" spans="1:6">
+      <c r="A672" t="s">
+        <v>89</v>
+      </c>
       <c r="B672">
         <v>18</v>
       </c>
@@ -11667,7 +12104,10 @@
         <v>416</v>
       </c>
     </row>
-    <row r="673" spans="2:6">
+    <row r="673" spans="1:6">
+      <c r="A673" t="s">
+        <v>89</v>
+      </c>
       <c r="B673">
         <v>21</v>
       </c>
@@ -11678,7 +12118,10 @@
         <v>418</v>
       </c>
     </row>
-    <row r="674" spans="2:6">
+    <row r="674" spans="1:6">
+      <c r="A674" t="s">
+        <v>89</v>
+      </c>
       <c r="B674">
         <v>25</v>
       </c>
@@ -11689,7 +12132,10 @@
         <v>419</v>
       </c>
     </row>
-    <row r="675" spans="2:6">
+    <row r="675" spans="1:6">
+      <c r="A675" t="s">
+        <v>89</v>
+      </c>
       <c r="B675">
         <v>28</v>
       </c>
@@ -11700,7 +12146,10 @@
         <v>420</v>
       </c>
     </row>
-    <row r="676" spans="2:6">
+    <row r="676" spans="1:6">
+      <c r="A676" t="s">
+        <v>89</v>
+      </c>
       <c r="B676">
         <v>31</v>
       </c>
@@ -11711,7 +12160,10 @@
         <v>421</v>
       </c>
     </row>
-    <row r="677" spans="2:6">
+    <row r="677" spans="1:6">
+      <c r="A677" t="s">
+        <v>89</v>
+      </c>
       <c r="B677">
         <v>35</v>
       </c>
@@ -11722,7 +12174,10 @@
         <v>422</v>
       </c>
     </row>
-    <row r="678" spans="2:6">
+    <row r="678" spans="1:6">
+      <c r="A678" t="s">
+        <v>89</v>
+      </c>
       <c r="B678">
         <v>38</v>
       </c>
@@ -11733,7 +12188,10 @@
         <v>423</v>
       </c>
     </row>
-    <row r="679" spans="2:6">
+    <row r="679" spans="1:6">
+      <c r="A679" t="s">
+        <v>89</v>
+      </c>
       <c r="B679">
         <v>42</v>
       </c>
@@ -11744,7 +12202,10 @@
         <v>424</v>
       </c>
     </row>
-    <row r="680" spans="2:6">
+    <row r="680" spans="1:6">
+      <c r="A680" t="s">
+        <v>89</v>
+      </c>
       <c r="B680">
         <v>45</v>
       </c>
@@ -11755,7 +12216,10 @@
         <v>425</v>
       </c>
     </row>
-    <row r="681" spans="2:6">
+    <row r="681" spans="1:6">
+      <c r="A681" t="s">
+        <v>89</v>
+      </c>
       <c r="B681">
         <v>48</v>
       </c>
@@ -11766,7 +12230,10 @@
         <v>426</v>
       </c>
     </row>
-    <row r="682" spans="2:6">
+    <row r="682" spans="1:6">
+      <c r="A682" t="s">
+        <v>89</v>
+      </c>
       <c r="B682">
         <v>52</v>
       </c>
@@ -11777,7 +12244,10 @@
         <v>427</v>
       </c>
     </row>
-    <row r="683" spans="2:6">
+    <row r="683" spans="1:6">
+      <c r="A683" t="s">
+        <v>89</v>
+      </c>
       <c r="B683">
         <v>59</v>
       </c>
@@ -11788,7 +12258,10 @@
         <v>428</v>
       </c>
     </row>
-    <row r="684" spans="2:6">
+    <row r="684" spans="1:6">
+      <c r="A684" t="s">
+        <v>89</v>
+      </c>
       <c r="B684">
         <v>62</v>
       </c>
@@ -11799,7 +12272,10 @@
         <v>429</v>
       </c>
     </row>
-    <row r="685" spans="2:6">
+    <row r="685" spans="1:6">
+      <c r="A685" t="s">
+        <v>89</v>
+      </c>
       <c r="B685">
         <v>65</v>
       </c>
@@ -11810,7 +12286,10 @@
         <v>430</v>
       </c>
     </row>
-    <row r="686" spans="2:6">
+    <row r="686" spans="1:6">
+      <c r="A686" t="s">
+        <v>89</v>
+      </c>
       <c r="B686">
         <v>69</v>
       </c>
@@ -11821,7 +12300,10 @@
         <v>503</v>
       </c>
     </row>
-    <row r="687" spans="2:6">
+    <row r="687" spans="1:6">
+      <c r="A687" t="s">
+        <v>89</v>
+      </c>
       <c r="B687">
         <v>72</v>
       </c>
@@ -11832,7 +12314,10 @@
         <v>504</v>
       </c>
     </row>
-    <row r="688" spans="2:6">
+    <row r="688" spans="1:6">
+      <c r="A688" t="s">
+        <v>89</v>
+      </c>
       <c r="B688">
         <v>76</v>
       </c>
@@ -11843,7 +12328,10 @@
         <v>432</v>
       </c>
     </row>
-    <row r="689" spans="2:6">
+    <row r="689" spans="1:6">
+      <c r="A689" t="s">
+        <v>89</v>
+      </c>
       <c r="B689">
         <v>79</v>
       </c>
@@ -11854,7 +12342,10 @@
         <v>434</v>
       </c>
     </row>
-    <row r="690" spans="2:6">
+    <row r="690" spans="1:6">
+      <c r="A690" t="s">
+        <v>89</v>
+      </c>
       <c r="B690">
         <v>82</v>
       </c>
@@ -11865,7 +12356,10 @@
         <v>505</v>
       </c>
     </row>
-    <row r="691" spans="2:6">
+    <row r="691" spans="1:6">
+      <c r="A691" t="s">
+        <v>89</v>
+      </c>
       <c r="B691">
         <v>86</v>
       </c>
@@ -11876,7 +12370,10 @@
         <v>506</v>
       </c>
     </row>
-    <row r="692" spans="2:6">
+    <row r="692" spans="1:6">
+      <c r="A692" t="s">
+        <v>89</v>
+      </c>
       <c r="B692">
         <v>89</v>
       </c>
@@ -11887,7 +12384,10 @@
         <v>507</v>
       </c>
     </row>
-    <row r="693" spans="2:6">
+    <row r="693" spans="1:6">
+      <c r="A693" t="s">
+        <v>89</v>
+      </c>
       <c r="B693">
         <v>93</v>
       </c>
@@ -11898,7 +12398,10 @@
         <v>508</v>
       </c>
     </row>
-    <row r="694" spans="2:6">
+    <row r="694" spans="1:6">
+      <c r="A694" t="s">
+        <v>89</v>
+      </c>
       <c r="B694">
         <v>96</v>
       </c>
@@ -11909,7 +12412,10 @@
         <v>509</v>
       </c>
     </row>
-    <row r="695" spans="2:6">
+    <row r="695" spans="1:6">
+      <c r="A695" t="s">
+        <v>89</v>
+      </c>
       <c r="B695">
         <v>99</v>
       </c>
@@ -11920,7 +12426,10 @@
         <v>510</v>
       </c>
     </row>
-    <row r="696" spans="2:6">
+    <row r="696" spans="1:6">
+      <c r="A696" t="s">
+        <v>89</v>
+      </c>
       <c r="B696">
         <v>22</v>
       </c>
@@ -11931,7 +12440,10 @@
         <v>437</v>
       </c>
     </row>
-    <row r="697" spans="2:6">
+    <row r="697" spans="1:6">
+      <c r="A697" t="s">
+        <v>89</v>
+      </c>
       <c r="B697">
         <v>49</v>
       </c>
@@ -11942,7 +12454,10 @@
         <v>438</v>
       </c>
     </row>
-    <row r="698" spans="2:6">
+    <row r="698" spans="1:6">
+      <c r="A698" t="s">
+        <v>89</v>
+      </c>
       <c r="B698">
         <v>70</v>
       </c>
@@ -11953,7 +12468,10 @@
         <v>511</v>
       </c>
     </row>
-    <row r="699" spans="2:6">
+    <row r="699" spans="1:6">
+      <c r="A699" t="s">
+        <v>89</v>
+      </c>
       <c r="B699">
         <v>43</v>
       </c>
@@ -11964,7 +12482,10 @@
         <v>439</v>
       </c>
     </row>
-    <row r="700" spans="2:6">
+    <row r="700" spans="1:6">
+      <c r="A700" t="s">
+        <v>89</v>
+      </c>
       <c r="B700">
         <v>36</v>
       </c>
@@ -11975,7 +12496,10 @@
         <v>440</v>
       </c>
     </row>
-    <row r="701" spans="2:6">
+    <row r="701" spans="1:6">
+      <c r="A701" t="s">
+        <v>89</v>
+      </c>
       <c r="B701">
         <v>2</v>
       </c>
@@ -11986,7 +12510,10 @@
         <v>441</v>
       </c>
     </row>
-    <row r="702" spans="2:6">
+    <row r="702" spans="1:6">
+      <c r="A702" t="s">
+        <v>89</v>
+      </c>
       <c r="B702">
         <v>90</v>
       </c>
@@ -11997,7 +12524,10 @@
         <v>442</v>
       </c>
     </row>
-    <row r="703" spans="2:6">
+    <row r="703" spans="1:6">
+      <c r="A703" t="s">
+        <v>89</v>
+      </c>
       <c r="B703">
         <v>56</v>
       </c>
@@ -12008,7 +12538,10 @@
         <v>444</v>
       </c>
     </row>
-    <row r="704" spans="2:6">
+    <row r="704" spans="1:6">
+      <c r="A704" t="s">
+        <v>89</v>
+      </c>
       <c r="B704">
         <v>15</v>
       </c>
@@ -12019,7 +12552,10 @@
         <v>445</v>
       </c>
     </row>
-    <row r="705" spans="2:6">
+    <row r="705" spans="1:6">
+      <c r="A705" t="s">
+        <v>89</v>
+      </c>
       <c r="B705">
         <v>83</v>
       </c>
@@ -12030,7 +12566,10 @@
         <v>512</v>
       </c>
     </row>
-    <row r="706" spans="2:6">
+    <row r="706" spans="1:6">
+      <c r="A706" t="s">
+        <v>89</v>
+      </c>
       <c r="B706">
         <v>9</v>
       </c>
@@ -12041,7 +12580,10 @@
         <v>446</v>
       </c>
     </row>
-    <row r="707" spans="2:6">
+    <row r="707" spans="1:6">
+      <c r="A707" t="s">
+        <v>89</v>
+      </c>
       <c r="B707">
         <v>29</v>
       </c>
@@ -12052,7 +12594,10 @@
         <v>447</v>
       </c>
     </row>
-    <row r="708" spans="2:6">
+    <row r="708" spans="1:6">
+      <c r="A708" t="s">
+        <v>89</v>
+      </c>
       <c r="B708">
         <v>97</v>
       </c>
@@ -12063,7 +12608,10 @@
         <v>530</v>
       </c>
     </row>
-    <row r="709" spans="2:6">
+    <row r="709" spans="1:6">
+      <c r="A709" t="s">
+        <v>89</v>
+      </c>
       <c r="B709">
         <v>77</v>
       </c>
@@ -12074,7 +12622,10 @@
         <v>449</v>
       </c>
     </row>
-    <row r="710" spans="2:6">
+    <row r="710" spans="1:6">
+      <c r="A710" t="s">
+        <v>89</v>
+      </c>
       <c r="B710">
         <v>63</v>
       </c>
@@ -12088,11 +12639,11 @@
   </sheetData>
   <autoFilter ref="A1:H47" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <phoneticPr fontId="7" type="noConversion"/>
+  <conditionalFormatting sqref="B30:B253 B260">
+    <cfRule type="duplicateValues" dxfId="3" priority="8"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B261:B274">
-    <cfRule type="duplicateValues" dxfId="3" priority="6"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B30:B253 B260">
-    <cfRule type="duplicateValues" dxfId="2" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="6"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -12103,7 +12654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -16197,7 +16748,7 @@
       <c r="L105"/>
       <c r="N105"/>
       <c r="O105"/>
-      <c r="Q105" s="28" t="s">
+      <c r="Q105" s="11" t="s">
         <v>519</v>
       </c>
       <c r="R105" s="22" t="s">
@@ -16653,7 +17204,7 @@
       <c r="L117"/>
       <c r="N117"/>
       <c r="O117"/>
-      <c r="Q117" s="28" t="s">
+      <c r="Q117" s="11" t="s">
         <v>521</v>
       </c>
       <c r="R117" s="17" t="s">
@@ -16805,7 +17356,7 @@
       <c r="L121"/>
       <c r="N121"/>
       <c r="O121"/>
-      <c r="Q121" s="28" t="s">
+      <c r="Q121" s="11" t="s">
         <v>521</v>
       </c>
       <c r="R121" s="17" t="s">
@@ -16843,7 +17394,7 @@
       <c r="L122"/>
       <c r="N122"/>
       <c r="O122"/>
-      <c r="Q122" s="28" t="s">
+      <c r="Q122" s="11" t="s">
         <v>521</v>
       </c>
       <c r="R122" s="17" t="s">
@@ -16881,7 +17432,7 @@
       <c r="L123"/>
       <c r="N123"/>
       <c r="O123"/>
-      <c r="Q123" s="28" t="s">
+      <c r="Q123" s="11" t="s">
         <v>521</v>
       </c>
       <c r="R123" s="17" t="s">
@@ -16919,7 +17470,7 @@
       <c r="L124"/>
       <c r="N124"/>
       <c r="O124"/>
-      <c r="Q124" s="28" t="s">
+      <c r="Q124" s="11" t="s">
         <v>521</v>
       </c>
       <c r="R124" s="17" t="s">
@@ -16957,7 +17508,7 @@
       <c r="L125"/>
       <c r="N125"/>
       <c r="O125"/>
-      <c r="Q125" s="28" t="s">
+      <c r="Q125" s="11" t="s">
         <v>521</v>
       </c>
       <c r="R125" s="17" t="s">
@@ -17071,7 +17622,7 @@
       <c r="L128"/>
       <c r="N128"/>
       <c r="O128"/>
-      <c r="Q128" s="28" t="s">
+      <c r="Q128" s="11" t="s">
         <v>521</v>
       </c>
       <c r="R128" s="17" t="s">
@@ -17147,7 +17698,7 @@
       <c r="L130"/>
       <c r="N130"/>
       <c r="O130"/>
-      <c r="Q130" s="28" t="s">
+      <c r="Q130" s="11" t="s">
         <v>521</v>
       </c>
       <c r="R130" s="17" t="s">
@@ -17185,7 +17736,7 @@
       <c r="L131"/>
       <c r="N131"/>
       <c r="O131"/>
-      <c r="Q131" s="28" t="s">
+      <c r="Q131" s="11" t="s">
         <v>521</v>
       </c>
       <c r="R131" s="17" t="s">
@@ -17261,7 +17812,7 @@
       <c r="L133"/>
       <c r="N133"/>
       <c r="O133"/>
-      <c r="Q133" s="28" t="s">
+      <c r="Q133" s="11" t="s">
         <v>521</v>
       </c>
       <c r="R133" s="17" t="s">
@@ -17375,7 +17926,7 @@
       <c r="L136"/>
       <c r="N136"/>
       <c r="O136"/>
-      <c r="Q136" s="28" t="s">
+      <c r="Q136" s="11" t="s">
         <v>521</v>
       </c>
       <c r="R136" s="17" t="s">
@@ -17451,7 +18002,7 @@
       <c r="L138"/>
       <c r="N138"/>
       <c r="O138"/>
-      <c r="Q138" s="28" t="s">
+      <c r="Q138" s="11" t="s">
         <v>521</v>
       </c>
       <c r="R138" s="17" t="s">
@@ -17489,7 +18040,7 @@
       <c r="L139"/>
       <c r="N139"/>
       <c r="O139"/>
-      <c r="Q139" s="28" t="s">
+      <c r="Q139" s="11" t="s">
         <v>521</v>
       </c>
       <c r="R139" s="17" t="s">
@@ -17565,7 +18116,7 @@
       <c r="L141"/>
       <c r="N141"/>
       <c r="O141"/>
-      <c r="Q141" s="28" t="s">
+      <c r="Q141" s="11" t="s">
         <v>521</v>
       </c>
       <c r="R141" s="17" t="s">
@@ -17755,7 +18306,7 @@
       <c r="L146"/>
       <c r="N146"/>
       <c r="O146"/>
-      <c r="Q146" s="28" t="s">
+      <c r="Q146" s="11" t="s">
         <v>521</v>
       </c>
       <c r="R146" s="17" t="s">
@@ -17793,7 +18344,7 @@
       <c r="L147"/>
       <c r="N147"/>
       <c r="O147"/>
-      <c r="Q147" s="28" t="s">
+      <c r="Q147" s="11" t="s">
         <v>521</v>
       </c>
       <c r="R147" s="17" t="s">
@@ -17831,7 +18382,7 @@
       <c r="L148"/>
       <c r="N148"/>
       <c r="O148"/>
-      <c r="Q148" s="28" t="s">
+      <c r="Q148" s="11" t="s">
         <v>521</v>
       </c>
       <c r="R148" s="17" t="s">
@@ -17869,7 +18420,7 @@
       <c r="L149"/>
       <c r="N149"/>
       <c r="O149"/>
-      <c r="Q149" s="28" t="s">
+      <c r="Q149" s="11" t="s">
         <v>521</v>
       </c>
       <c r="R149" s="17" t="s">
@@ -17907,7 +18458,7 @@
       <c r="L150"/>
       <c r="N150"/>
       <c r="O150"/>
-      <c r="Q150" s="28" t="s">
+      <c r="Q150" s="11" t="s">
         <v>521</v>
       </c>
       <c r="R150" s="17" t="s">
@@ -18097,7 +18648,7 @@
       <c r="L155"/>
       <c r="N155"/>
       <c r="O155"/>
-      <c r="Q155" s="28" t="s">
+      <c r="Q155" s="11" t="s">
         <v>521</v>
       </c>
       <c r="R155" s="17" t="s">
@@ -18135,7 +18686,7 @@
       <c r="L156"/>
       <c r="N156"/>
       <c r="O156"/>
-      <c r="Q156" s="28" t="s">
+      <c r="Q156" s="11" t="s">
         <v>521</v>
       </c>
       <c r="R156" s="17" t="s">
@@ -18211,7 +18762,7 @@
       <c r="L158"/>
       <c r="N158"/>
       <c r="O158"/>
-      <c r="Q158" s="28" t="s">
+      <c r="Q158" s="11" t="s">
         <v>523</v>
       </c>
       <c r="R158" s="17" t="s">
@@ -18480,7 +19031,7 @@
       <c r="Q165" s="11" t="s">
         <v>523</v>
       </c>
-      <c r="R165" s="28" t="s">
+      <c r="R165" s="11" t="s">
         <v>504</v>
       </c>
     </row>
@@ -18518,7 +19069,7 @@
       <c r="Q166" s="11" t="s">
         <v>523</v>
       </c>
-      <c r="R166" s="28" t="s">
+      <c r="R166" s="11" t="s">
         <v>422</v>
       </c>
     </row>
@@ -18974,7 +19525,7 @@
       <c r="Q178" s="11" t="s">
         <v>523</v>
       </c>
-      <c r="R178" s="28" t="s">
+      <c r="R178" s="11" t="s">
         <v>511</v>
       </c>
     </row>
@@ -19883,7 +20434,7 @@
       <c r="L202"/>
       <c r="N202"/>
       <c r="O202"/>
-      <c r="Q202" s="28" t="s">
+      <c r="Q202" s="11" t="s">
         <v>520</v>
       </c>
       <c r="R202" s="17" t="s">
@@ -19921,7 +20472,7 @@
       <c r="L203"/>
       <c r="N203"/>
       <c r="O203"/>
-      <c r="Q203" s="28" t="s">
+      <c r="Q203" s="11" t="s">
         <v>520</v>
       </c>
       <c r="R203" s="22" t="s">
@@ -19959,7 +20510,7 @@
       <c r="L204"/>
       <c r="N204"/>
       <c r="O204"/>
-      <c r="Q204" s="28" t="s">
+      <c r="Q204" s="11" t="s">
         <v>520</v>
       </c>
       <c r="R204" s="17" t="s">
@@ -19997,7 +20548,7 @@
       <c r="L205"/>
       <c r="N205"/>
       <c r="O205"/>
-      <c r="Q205" s="28" t="s">
+      <c r="Q205" s="11" t="s">
         <v>520</v>
       </c>
       <c r="R205" s="22" t="s">
@@ -20035,7 +20586,7 @@
       <c r="L206"/>
       <c r="N206"/>
       <c r="O206"/>
-      <c r="Q206" s="28" t="s">
+      <c r="Q206" s="11" t="s">
         <v>520</v>
       </c>
       <c r="R206" s="22" t="s">
@@ -20073,7 +20624,7 @@
       <c r="L207"/>
       <c r="N207"/>
       <c r="O207"/>
-      <c r="Q207" s="28" t="s">
+      <c r="Q207" s="11" t="s">
         <v>520</v>
       </c>
       <c r="R207" s="17" t="s">
@@ -20111,7 +20662,7 @@
       <c r="L208"/>
       <c r="N208"/>
       <c r="O208"/>
-      <c r="Q208" s="28" t="s">
+      <c r="Q208" s="11" t="s">
         <v>520</v>
       </c>
       <c r="R208" s="22" t="s">
@@ -20149,7 +20700,7 @@
       <c r="L209"/>
       <c r="N209"/>
       <c r="O209"/>
-      <c r="Q209" s="28" t="s">
+      <c r="Q209" s="11" t="s">
         <v>520</v>
       </c>
       <c r="R209" s="22" t="s">
@@ -20187,7 +20738,7 @@
       <c r="L210"/>
       <c r="N210"/>
       <c r="O210"/>
-      <c r="Q210" s="28" t="s">
+      <c r="Q210" s="11" t="s">
         <v>520</v>
       </c>
       <c r="R210" s="22" t="s">
@@ -20225,7 +20776,7 @@
       <c r="L211"/>
       <c r="N211"/>
       <c r="O211"/>
-      <c r="Q211" s="28" t="s">
+      <c r="Q211" s="11" t="s">
         <v>520</v>
       </c>
       <c r="R211" s="17" t="s">
@@ -20263,7 +20814,7 @@
       <c r="L212"/>
       <c r="N212"/>
       <c r="O212"/>
-      <c r="Q212" s="28" t="s">
+      <c r="Q212" s="11" t="s">
         <v>520</v>
       </c>
       <c r="R212" s="17" t="s">
@@ -20301,7 +20852,7 @@
       <c r="L213"/>
       <c r="N213"/>
       <c r="O213"/>
-      <c r="Q213" s="28" t="s">
+      <c r="Q213" s="11" t="s">
         <v>520</v>
       </c>
       <c r="R213" s="22" t="s">
@@ -20339,7 +20890,7 @@
       <c r="L214"/>
       <c r="N214"/>
       <c r="O214"/>
-      <c r="Q214" s="28" t="s">
+      <c r="Q214" s="11" t="s">
         <v>520</v>
       </c>
       <c r="R214" s="22" t="s">
@@ -20377,7 +20928,7 @@
       <c r="L215"/>
       <c r="N215"/>
       <c r="O215"/>
-      <c r="Q215" s="28" t="s">
+      <c r="Q215" s="11" t="s">
         <v>520</v>
       </c>
       <c r="R215" s="22" t="s">
@@ -20415,7 +20966,7 @@
       <c r="L216"/>
       <c r="N216"/>
       <c r="O216"/>
-      <c r="Q216" s="28" t="s">
+      <c r="Q216" s="11" t="s">
         <v>520</v>
       </c>
       <c r="R216" s="22" t="s">
@@ -20453,7 +21004,7 @@
       <c r="L217"/>
       <c r="N217"/>
       <c r="O217"/>
-      <c r="Q217" s="28" t="s">
+      <c r="Q217" s="11" t="s">
         <v>520</v>
       </c>
       <c r="R217" s="17" t="s">
@@ -20491,7 +21042,7 @@
       <c r="L218"/>
       <c r="N218"/>
       <c r="O218"/>
-      <c r="Q218" s="28" t="s">
+      <c r="Q218" s="11" t="s">
         <v>520</v>
       </c>
       <c r="R218" s="22" t="s">
@@ -20529,7 +21080,7 @@
       <c r="L219"/>
       <c r="N219"/>
       <c r="O219"/>
-      <c r="Q219" s="28" t="s">
+      <c r="Q219" s="11" t="s">
         <v>520</v>
       </c>
       <c r="R219" s="22" t="s">
@@ -20567,7 +21118,7 @@
       <c r="L220"/>
       <c r="N220"/>
       <c r="O220"/>
-      <c r="Q220" s="28" t="s">
+      <c r="Q220" s="11" t="s">
         <v>520</v>
       </c>
       <c r="R220" s="22" t="s">
@@ -20605,7 +21156,7 @@
       <c r="L221"/>
       <c r="N221"/>
       <c r="O221"/>
-      <c r="Q221" s="28" t="s">
+      <c r="Q221" s="11" t="s">
         <v>520</v>
       </c>
       <c r="R221" s="17" t="s">
@@ -20643,7 +21194,7 @@
       <c r="L222"/>
       <c r="N222"/>
       <c r="O222"/>
-      <c r="Q222" s="28" t="s">
+      <c r="Q222" s="11" t="s">
         <v>520</v>
       </c>
       <c r="R222" s="22" t="s">
@@ -20681,7 +21232,7 @@
       <c r="L223"/>
       <c r="N223"/>
       <c r="O223"/>
-      <c r="Q223" s="28" t="s">
+      <c r="Q223" s="11" t="s">
         <v>520</v>
       </c>
       <c r="R223" s="22" t="s">
@@ -20719,7 +21270,7 @@
       <c r="L224"/>
       <c r="N224"/>
       <c r="O224"/>
-      <c r="Q224" s="28" t="s">
+      <c r="Q224" s="11" t="s">
         <v>520</v>
       </c>
       <c r="R224" s="22" t="s">
@@ -20757,7 +21308,7 @@
       <c r="L225"/>
       <c r="N225"/>
       <c r="O225"/>
-      <c r="Q225" s="28" t="s">
+      <c r="Q225" s="11" t="s">
         <v>520</v>
       </c>
       <c r="R225" s="22" t="s">

</xml_diff>